<commit_message>
Prep work to add support for sub-products
</commit_message>
<xml_diff>
--- a/input_data/8001/cli.post_dry_run/pbf_opus.update.big-rocks.journeys.a6i.xlsx
+++ b/input_data/8001/cli.post_dry_run/pbf_opus.update.big-rocks.journeys.a6i.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\test_db\input_data\8001\cli.post_by_file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\test_db\input_data\8001\cli.post_dry_run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396F1616-9597-462D-8B4A-4C71454D9CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13251C78-A729-4387-9F03-66C6EE48001C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Posting Label" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>variant</t>
   </si>
   <si>
-    <t>priorVersion.1</t>
-  </si>
-  <si>
     <t>priorVersion.2</t>
   </si>
   <si>
@@ -91,15 +88,6 @@
     <t>data.sheet.0</t>
   </si>
   <si>
-    <t>data.kind.1</t>
-  </si>
-  <si>
-    <t>data.range.1</t>
-  </si>
-  <si>
-    <t>data.sheet.1</t>
-  </si>
-  <si>
     <t>data.kind.2</t>
   </si>
   <si>
@@ -260,6 +248,18 @@
   </si>
   <si>
     <t>Modernization – Persona Based Dashboard, Improved UI/UX -*CHANGED</t>
+  </si>
+  <si>
+    <t>data.kind.3</t>
+  </si>
+  <si>
+    <t>data.range.3</t>
+  </si>
+  <si>
+    <t>data.sheet.3</t>
+  </si>
+  <si>
+    <t>priorVersion.3</t>
   </si>
 </sst>
 </file>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -743,7 +743,7 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
@@ -751,7 +751,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
@@ -759,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
@@ -767,7 +767,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
@@ -775,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
@@ -783,7 +783,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
@@ -807,7 +807,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.45">
@@ -815,7 +815,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.45">
@@ -823,7 +823,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
@@ -831,7 +831,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
@@ -839,7 +839,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
@@ -847,7 +847,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
@@ -855,7 +855,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.45">
@@ -868,7 +868,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -876,78 +876,78 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B25" s="2" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B26" s="2" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -956,7 +956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -972,57 +972,57 @@
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="J2" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="7">
         <v>2000</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I3" s="7">
         <v>3584</v>
@@ -1036,14 +1036,14 @@
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="7">
         <v>2050</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I4" s="7">
         <v>5207</v>
@@ -1055,20 +1055,20 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="7">
         <v>6600</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I5" s="7">
         <v>5575</v>
@@ -1083,13 +1083,13 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F6" s="7">
         <v>600</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I6" s="7">
         <v>5800</v>
@@ -1103,14 +1103,14 @@
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="7">
         <v>3000</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I7" s="7">
         <v>5860</v>
@@ -1122,10 +1122,10 @@
     </row>
     <row r="8" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1133,7 +1133,7 @@
         <v>4500</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I8" s="7">
         <v>3600</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1157,10 +1157,10 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C11" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>

</xml_diff>